<commit_message>
update phi nhap hang theo thang
</commit_message>
<xml_diff>
--- a/Ke hoach ban hang.xlsx
+++ b/Ke hoach ban hang.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="104">
   <si>
     <t>Tháng 1</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Tổng doanh thu bán hàng theo tháng</t>
+  </si>
+  <si>
+    <t>Tổng Tiền nhập sản phẩm theo từng tháng</t>
+  </si>
+  <si>
+    <t>Tính tiền nhập sản phẩm</t>
   </si>
 </sst>
 </file>
@@ -399,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -595,13 +601,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -666,6 +681,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -978,7 +997,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,15 +1218,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -1217,7 +1236,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1270,7 +1289,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="2">
@@ -1326,7 +1345,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="2">
@@ -1382,7 +1401,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="2">
@@ -1438,7 +1457,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2">
@@ -1494,7 +1513,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
@@ -1550,7 +1569,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2">
@@ -1606,7 +1625,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2">
@@ -1662,7 +1681,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2">
@@ -1718,7 +1737,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2">
@@ -1774,7 +1793,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B11" s="2">
@@ -1838,7 +1857,676 @@
         <v>192200</v>
       </c>
     </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+    </row>
+    <row r="14" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="str">
+        <f t="shared" ref="A14:M14" si="3">A1</f>
+        <v>Sản phẩm</v>
+      </c>
+      <c r="B14" s="17" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 1</v>
+      </c>
+      <c r="C14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 2</v>
+      </c>
+      <c r="D14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 3</v>
+      </c>
+      <c r="E14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 4</v>
+      </c>
+      <c r="F14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 5</v>
+      </c>
+      <c r="G14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 6</v>
+      </c>
+      <c r="H14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 7</v>
+      </c>
+      <c r="I14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 8</v>
+      </c>
+      <c r="J14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 9</v>
+      </c>
+      <c r="K14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 10</v>
+      </c>
+      <c r="L14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 11</v>
+      </c>
+      <c r="M14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>Tháng 12</v>
+      </c>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="str">
+        <f t="shared" ref="A15:M15" si="4">A2</f>
+        <v>Dịch vụ Sửa PC</v>
+      </c>
+      <c r="B15" s="18">
+        <f>B2*$P2</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="18">
+        <f t="shared" ref="C15:M15" si="5">C2*$P2</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="str">
+        <f t="shared" ref="A16:M16" si="6">A3</f>
+        <v>Dịch vụ Sửa Laptop</v>
+      </c>
+      <c r="B16" s="18">
+        <f>B3*$P3</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="18">
+        <f t="shared" ref="C16:M16" si="7">C3*$P3</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="str">
+        <f t="shared" ref="A17:M17" si="8">A4</f>
+        <v>PC (bán)</v>
+      </c>
+      <c r="B17" s="18">
+        <f>B4*$P4</f>
+        <v>16000</v>
+      </c>
+      <c r="C17" s="18">
+        <f t="shared" ref="C17:M17" si="9">C4*$P4</f>
+        <v>64000</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" si="9"/>
+        <v>56000</v>
+      </c>
+      <c r="E17" s="18">
+        <f t="shared" si="9"/>
+        <v>80000</v>
+      </c>
+      <c r="F17" s="18">
+        <f t="shared" si="9"/>
+        <v>80000</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="9"/>
+        <v>72000</v>
+      </c>
+      <c r="H17" s="18">
+        <f t="shared" si="9"/>
+        <v>40000</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="9"/>
+        <v>88000</v>
+      </c>
+      <c r="J17" s="18">
+        <f t="shared" si="9"/>
+        <v>96000</v>
+      </c>
+      <c r="K17" s="18">
+        <f t="shared" si="9"/>
+        <v>120000</v>
+      </c>
+      <c r="L17" s="18">
+        <f t="shared" si="9"/>
+        <v>56000</v>
+      </c>
+      <c r="M17" s="18">
+        <f t="shared" si="9"/>
+        <v>64000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="str">
+        <f t="shared" ref="A18:M18" si="10">A5</f>
+        <v>Ram</v>
+      </c>
+      <c r="B18" s="18">
+        <f>B5*$P5</f>
+        <v>4500</v>
+      </c>
+      <c r="C18" s="18">
+        <f t="shared" ref="C18:M18" si="11">C5*$P5</f>
+        <v>13500</v>
+      </c>
+      <c r="D18" s="18">
+        <f t="shared" si="11"/>
+        <v>18000</v>
+      </c>
+      <c r="E18" s="18">
+        <f t="shared" si="11"/>
+        <v>15300</v>
+      </c>
+      <c r="F18" s="18">
+        <f t="shared" si="11"/>
+        <v>18000</v>
+      </c>
+      <c r="G18" s="18">
+        <f t="shared" si="11"/>
+        <v>19800</v>
+      </c>
+      <c r="H18" s="18">
+        <f t="shared" si="11"/>
+        <v>14400</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="11"/>
+        <v>16200</v>
+      </c>
+      <c r="J18" s="18">
+        <f t="shared" si="11"/>
+        <v>13500</v>
+      </c>
+      <c r="K18" s="18">
+        <f t="shared" si="11"/>
+        <v>15300</v>
+      </c>
+      <c r="L18" s="18">
+        <f t="shared" si="11"/>
+        <v>9000</v>
+      </c>
+      <c r="M18" s="18">
+        <f t="shared" si="11"/>
+        <v>11700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="str">
+        <f t="shared" ref="A19:M19" si="12">A6</f>
+        <v>Ổ cứng</v>
+      </c>
+      <c r="B19" s="18">
+        <f>B6*$P6</f>
+        <v>2500</v>
+      </c>
+      <c r="C19" s="18">
+        <f t="shared" ref="C19:M19" si="13">C6*$P6</f>
+        <v>25000</v>
+      </c>
+      <c r="D19" s="18">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="E19" s="18">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="F19" s="18">
+        <f t="shared" si="13"/>
+        <v>17500</v>
+      </c>
+      <c r="G19" s="18">
+        <f t="shared" si="13"/>
+        <v>22500</v>
+      </c>
+      <c r="H19" s="18">
+        <f t="shared" si="13"/>
+        <v>2500</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="J19" s="18">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="K19" s="18">
+        <f t="shared" si="13"/>
+        <v>25000</v>
+      </c>
+      <c r="L19" s="18">
+        <f t="shared" si="13"/>
+        <v>17500</v>
+      </c>
+      <c r="M19" s="18">
+        <f t="shared" si="13"/>
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="str">
+        <f t="shared" ref="A20:M20" si="14">A7</f>
+        <v>bàn phím/chuột</v>
+      </c>
+      <c r="B20" s="18">
+        <f>B7*$P7</f>
+        <v>3000</v>
+      </c>
+      <c r="C20" s="18">
+        <f t="shared" ref="C20:M20" si="15">C7*$P7</f>
+        <v>9000</v>
+      </c>
+      <c r="D20" s="18">
+        <f t="shared" si="15"/>
+        <v>15000</v>
+      </c>
+      <c r="E20" s="18">
+        <f t="shared" si="15"/>
+        <v>13500</v>
+      </c>
+      <c r="F20" s="18">
+        <f t="shared" si="15"/>
+        <v>15000</v>
+      </c>
+      <c r="G20" s="18">
+        <f t="shared" si="15"/>
+        <v>16800</v>
+      </c>
+      <c r="H20" s="18">
+        <f t="shared" si="15"/>
+        <v>16500</v>
+      </c>
+      <c r="I20" s="18">
+        <f t="shared" si="15"/>
+        <v>16800</v>
+      </c>
+      <c r="J20" s="18">
+        <f t="shared" si="15"/>
+        <v>13200</v>
+      </c>
+      <c r="K20" s="18">
+        <f t="shared" si="15"/>
+        <v>13500</v>
+      </c>
+      <c r="L20" s="18">
+        <f t="shared" si="15"/>
+        <v>15000</v>
+      </c>
+      <c r="M20" s="18">
+        <f t="shared" si="15"/>
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="str">
+        <f t="shared" ref="A21:M21" si="16">A8</f>
+        <v>Màn hình</v>
+      </c>
+      <c r="B21" s="18">
+        <f>B8*$P8</f>
+        <v>6000</v>
+      </c>
+      <c r="C21" s="18">
+        <f t="shared" ref="C21:M21" si="17">C8*$P8</f>
+        <v>18000</v>
+      </c>
+      <c r="D21" s="18">
+        <f t="shared" si="17"/>
+        <v>30000</v>
+      </c>
+      <c r="E21" s="18">
+        <f t="shared" si="17"/>
+        <v>27000</v>
+      </c>
+      <c r="F21" s="18">
+        <f t="shared" si="17"/>
+        <v>33000</v>
+      </c>
+      <c r="G21" s="18">
+        <f t="shared" si="17"/>
+        <v>36000</v>
+      </c>
+      <c r="H21" s="18">
+        <f t="shared" si="17"/>
+        <v>24000</v>
+      </c>
+      <c r="I21" s="18">
+        <f t="shared" si="17"/>
+        <v>30000</v>
+      </c>
+      <c r="J21" s="18">
+        <f t="shared" si="17"/>
+        <v>33000</v>
+      </c>
+      <c r="K21" s="18">
+        <f t="shared" si="17"/>
+        <v>27000</v>
+      </c>
+      <c r="L21" s="18">
+        <f t="shared" si="17"/>
+        <v>21000</v>
+      </c>
+      <c r="M21" s="18">
+        <f t="shared" si="17"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="str">
+        <f t="shared" ref="A22:M22" si="18">A9</f>
+        <v>USB</v>
+      </c>
+      <c r="B22" s="18">
+        <f>B9*$P9</f>
+        <v>1400</v>
+      </c>
+      <c r="C22" s="18">
+        <f t="shared" ref="C22:M22" si="19">C9*$P9</f>
+        <v>4400</v>
+      </c>
+      <c r="D22" s="18">
+        <f t="shared" si="19"/>
+        <v>6000</v>
+      </c>
+      <c r="E22" s="18">
+        <f t="shared" si="19"/>
+        <v>4800</v>
+      </c>
+      <c r="F22" s="18">
+        <f t="shared" si="19"/>
+        <v>6200</v>
+      </c>
+      <c r="G22" s="18">
+        <f t="shared" si="19"/>
+        <v>7000</v>
+      </c>
+      <c r="H22" s="18">
+        <f t="shared" si="19"/>
+        <v>5600</v>
+      </c>
+      <c r="I22" s="18">
+        <f t="shared" si="19"/>
+        <v>5000</v>
+      </c>
+      <c r="J22" s="18">
+        <f t="shared" si="19"/>
+        <v>6000</v>
+      </c>
+      <c r="K22" s="18">
+        <f t="shared" si="19"/>
+        <v>6600</v>
+      </c>
+      <c r="L22" s="18">
+        <f t="shared" si="19"/>
+        <v>6200</v>
+      </c>
+      <c r="M22" s="18">
+        <f t="shared" si="19"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="str">
+        <f t="shared" ref="A23:M23" si="20">A10</f>
+        <v>Mainboard</v>
+      </c>
+      <c r="B23" s="18">
+        <f>B10*$P10</f>
+        <v>2500</v>
+      </c>
+      <c r="C23" s="18">
+        <f t="shared" ref="C23:M23" si="21">C10*$P10</f>
+        <v>12500</v>
+      </c>
+      <c r="D23" s="18">
+        <f t="shared" si="21"/>
+        <v>12500</v>
+      </c>
+      <c r="E23" s="18">
+        <f t="shared" si="21"/>
+        <v>12500</v>
+      </c>
+      <c r="F23" s="18">
+        <f t="shared" si="21"/>
+        <v>15000</v>
+      </c>
+      <c r="G23" s="18">
+        <f t="shared" si="21"/>
+        <v>22500</v>
+      </c>
+      <c r="H23" s="18">
+        <f t="shared" si="21"/>
+        <v>15000</v>
+      </c>
+      <c r="I23" s="18">
+        <f t="shared" si="21"/>
+        <v>20000</v>
+      </c>
+      <c r="J23" s="18">
+        <f t="shared" si="21"/>
+        <v>20000</v>
+      </c>
+      <c r="K23" s="18">
+        <f t="shared" si="21"/>
+        <v>17500</v>
+      </c>
+      <c r="L23" s="18">
+        <f t="shared" si="21"/>
+        <v>15000</v>
+      </c>
+      <c r="M23" s="18">
+        <f t="shared" si="21"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="str">
+        <f t="shared" ref="A24:M24" si="22">A11</f>
+        <v>Linh kiện khác (Nguồn, quạt tản nhiệt, GPU,….vv)</v>
+      </c>
+      <c r="B24" s="18">
+        <f>B11*$P11</f>
+        <v>25000</v>
+      </c>
+      <c r="C24" s="18">
+        <f t="shared" ref="C24:M24" si="23">C11*$P11</f>
+        <v>47500</v>
+      </c>
+      <c r="D24" s="18">
+        <f t="shared" si="23"/>
+        <v>50000</v>
+      </c>
+      <c r="E24" s="18">
+        <f t="shared" si="23"/>
+        <v>42500</v>
+      </c>
+      <c r="F24" s="18">
+        <f t="shared" si="23"/>
+        <v>45000</v>
+      </c>
+      <c r="G24" s="18">
+        <f t="shared" si="23"/>
+        <v>47500</v>
+      </c>
+      <c r="H24" s="18">
+        <f t="shared" si="23"/>
+        <v>42500</v>
+      </c>
+      <c r="I24" s="18">
+        <f t="shared" si="23"/>
+        <v>47500</v>
+      </c>
+      <c r="J24" s="18">
+        <f t="shared" si="23"/>
+        <v>40000</v>
+      </c>
+      <c r="K24" s="18">
+        <f t="shared" si="23"/>
+        <v>50000</v>
+      </c>
+      <c r="L24" s="18">
+        <f t="shared" si="23"/>
+        <v>45000</v>
+      </c>
+      <c r="M24" s="18">
+        <f t="shared" si="23"/>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="20">
+        <f>SUM(B15:B24)</f>
+        <v>60900</v>
+      </c>
+      <c r="C25" s="20">
+        <f t="shared" ref="C25:M25" si="24">SUM(C15:C24)</f>
+        <v>193900</v>
+      </c>
+      <c r="D25" s="20">
+        <f t="shared" si="24"/>
+        <v>212500</v>
+      </c>
+      <c r="E25" s="20">
+        <f t="shared" si="24"/>
+        <v>220600</v>
+      </c>
+      <c r="F25" s="20">
+        <f t="shared" si="24"/>
+        <v>229700</v>
+      </c>
+      <c r="G25" s="20">
+        <f t="shared" si="24"/>
+        <v>244100</v>
+      </c>
+      <c r="H25" s="20">
+        <f t="shared" si="24"/>
+        <v>160500</v>
+      </c>
+      <c r="I25" s="20">
+        <f t="shared" si="24"/>
+        <v>248500</v>
+      </c>
+      <c r="J25" s="20">
+        <f t="shared" si="24"/>
+        <v>246700</v>
+      </c>
+      <c r="K25" s="20">
+        <f t="shared" si="24"/>
+        <v>274900</v>
+      </c>
+      <c r="L25" s="20">
+        <f t="shared" si="24"/>
+        <v>184700</v>
+      </c>
+      <c r="M25" s="20">
+        <f t="shared" si="24"/>
+        <v>173200</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A13:M13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2090,7 +2778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -2651,7 +3339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>

</xml_diff>